<commit_message>
updating test cases excel file
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
+++ b/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7806B7E2-DB9B-4A92-A531-8E3069032EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B326D33-3896-48DC-B619-EF8E5576CF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="120">
   <si>
     <t>Comments</t>
   </si>
@@ -1213,6 +1213,24 @@
   </si>
   <si>
     <t>Multiple comma delimited phrases have been correctly identified, separated, and displayed with the appropriate positional value.</t>
+  </si>
+  <si>
+    <t>Trying negative values</t>
+  </si>
+  <si>
+    <t>123456789ab</t>
+  </si>
+  <si>
+    <t>trying to enter values with character</t>
+  </si>
+  <si>
+    <t>The programs ends with the end message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To see if the programs ends </t>
+  </si>
+  <si>
+    <t>Trying the edge values</t>
   </si>
 </sst>
 </file>
@@ -1760,7 +1778,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1771,9 +1789,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1783,9 +1798,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1794,9 +1806,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1893,12 +1902,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1911,59 +1959,41 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2254,95 +2284,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
-  <dimension ref="A1:I68"/>
+  <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="59" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="C66" sqref="C66"/>
+    <sheetView tabSelected="1" topLeftCell="D56" zoomScale="115" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="49" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="str" cm="1">
+      <c r="B1" s="16" t="str" cm="1">
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="65" t="s">
+      <c r="C1" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-    </row>
-    <row r="2" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="63" t="s">
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="26" t="s">
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="F3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G4" s="3" t="s">
@@ -2351,22 +2381,22 @@
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G5" s="3" t="s">
@@ -2375,47 +2405,47 @@
       <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="18"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -2424,22 +2454,22 @@
       <c r="I7" s="2"/>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="E8" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -2448,22 +2478,22 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="12" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="3" t="s">
@@ -2472,1146 +2502,1217 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6">
         <v>123456</v>
       </c>
-      <c r="D10" s="67" t="s">
+      <c r="D10" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="54" t="s">
+      <c r="F10" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="59" t="s">
+      <c r="G10" s="47" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
     </row>
     <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="5">
+      <c r="A11" s="11"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="4">
         <v>7891011</v>
       </c>
-      <c r="D11" s="68"/>
-      <c r="E11" s="71"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="60"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="48"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="67" t="s">
+      <c r="D12" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="54" t="s">
+      <c r="F12" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="59" t="s">
+      <c r="G12" s="47" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
     </row>
     <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="18" t="s">
+      <c r="A13" s="11"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="68"/>
-      <c r="E13" s="71"/>
-      <c r="F13" s="55"/>
-      <c r="G13" s="60"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="59"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="48"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="67" t="s">
+      <c r="D14" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="70" t="s">
+      <c r="E14" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="54" t="s">
+      <c r="F14" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="59" t="s">
+      <c r="G14" s="47" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="5" t="s">
+      <c r="A15" s="11"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="68"/>
-      <c r="E15" s="71"/>
-      <c r="F15" s="55"/>
-      <c r="G15" s="60"/>
+      <c r="D15" s="56"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="48"/>
       <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="69" t="s">
+      <c r="D16" s="57" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="59" t="s">
+      <c r="E16" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="54" t="s">
+      <c r="F16" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="49" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7" t="s">
+      <c r="A17" s="11"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="49"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="48"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="50"/>
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="48" t="s">
+      <c r="C18" s="6"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="54" t="s">
+      <c r="F18" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="59" t="s">
+      <c r="G18" s="47" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="68"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="60"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="48"/>
       <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="67" t="s">
+      <c r="D20" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="54" t="s">
+      <c r="F20" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="59" t="s">
+      <c r="G20" s="47" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
     <row r="21" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="68"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="60"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="56"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="48"/>
       <c r="I21" s="1"/>
     </row>
     <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="33" t="s">
+      <c r="C22" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="31" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G22" s="16" t="s">
+      <c r="G22" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I22" s="1"/>
     </row>
     <row r="23" spans="1:9" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="16" t="s">
+      <c r="G23" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I23" s="1"/>
     </row>
     <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="14" t="s">
+      <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="16" t="s">
+      <c r="G24" s="13" t="s">
         <v>35</v>
       </c>
       <c r="I24" s="2"/>
     </row>
     <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="14" t="s">
+      <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="29">
+      <c r="D25" s="26">
         <v>123</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="29" t="s">
         <v>62</v>
       </c>
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="14" t="s">
+      <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="26">
         <v>0</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G26" s="32" t="s">
+      <c r="G26" s="29" t="s">
         <v>63</v>
       </c>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="D27" s="29">
+      <c r="D27" s="26">
         <v>123</v>
       </c>
-      <c r="E27" s="16">
+      <c r="E27" s="13">
         <v>12332</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="29" t="s">
         <v>64</v>
       </c>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="26">
         <v>0</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="32" t="s">
+      <c r="G28" s="29" t="s">
         <v>65</v>
       </c>
       <c r="I28" s="2"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="26">
         <v>0</v>
       </c>
-      <c r="E29" s="16">
+      <c r="E29" s="13">
         <v>1246</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="29" t="s">
         <v>66</v>
       </c>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="27" t="s">
         <v>59</v>
       </c>
-      <c r="D30" s="29">
+      <c r="D30" s="26">
         <v>12</v>
       </c>
-      <c r="E30" s="16" t="s">
+      <c r="E30" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="32" t="s">
+      <c r="G30" s="29" t="s">
         <v>64</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="29">
+      <c r="D31" s="26">
         <v>0</v>
       </c>
-      <c r="E31" s="16">
+      <c r="E31" s="13">
         <v>122</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="29" t="s">
         <v>62</v>
       </c>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="13" t="s">
+      <c r="B32" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="D32" s="29" t="s">
+      <c r="D32" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="16" t="s">
+      <c r="E32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G32" s="32" t="s">
+      <c r="G32" s="29" t="s">
         <v>64</v>
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" s="9" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="63" t="s">
+    <row r="33" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="51" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="26" t="s">
+      <c r="B33" s="52"/>
+      <c r="C33" s="52"/>
+      <c r="D33" s="52"/>
+      <c r="E33" s="52"/>
+      <c r="F33" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="28" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="22" t="s">
+      <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="24" t="s">
+      <c r="C34" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D34" s="24" t="s">
+      <c r="D34" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E34" s="24" t="s">
+      <c r="E34" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="9" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="E35" s="40" t="s">
+      <c r="E35" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G35" s="16" t="s">
+      <c r="G35" s="13" t="s">
         <v>93</v>
       </c>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="36" t="s">
+      <c r="C36" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="E36" s="40" t="s">
+      <c r="E36" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="16" t="s">
+      <c r="G36" s="13" t="s">
         <v>93</v>
       </c>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="40" t="s">
+      <c r="E37" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G37" s="13" t="s">
         <v>93</v>
       </c>
       <c r="I37" s="1"/>
     </row>
     <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="50" t="s">
+      <c r="A38" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="52" t="s">
+      <c r="B38" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="56" t="s">
+      <c r="D38" s="64" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="48" t="s">
+      <c r="E38" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="54" t="s">
+      <c r="F38" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="59" t="s">
+      <c r="G38" s="47" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="51"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="7">
+      <c r="A39" s="61"/>
+      <c r="B39" s="63"/>
+      <c r="C39" s="6">
         <v>3</v>
       </c>
-      <c r="D39" s="62"/>
-      <c r="E39" s="49"/>
-      <c r="F39" s="55"/>
-      <c r="G39" s="60"/>
+      <c r="D39" s="65"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="48"/>
       <c r="I39" s="1"/>
     </row>
     <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="50" t="s">
+      <c r="A40" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="52" t="s">
+      <c r="B40" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="48" t="s">
+      <c r="E40" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="54" t="s">
+      <c r="F40" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="59" t="s">
+      <c r="G40" s="47" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
     <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="51"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="7" t="s">
+      <c r="A41" s="61"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="62"/>
-      <c r="E41" s="49"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="60"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="48"/>
       <c r="I41" s="1"/>
     </row>
     <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="50" t="s">
+      <c r="A42" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="52" t="s">
+      <c r="B42" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="61" t="s">
+      <c r="D42" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="48" t="s">
+      <c r="E42" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="54" t="s">
+      <c r="F42" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="48" t="s">
+      <c r="G42" s="49" t="s">
         <v>81</v>
       </c>
       <c r="I42" s="1"/>
     </row>
     <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="51"/>
-      <c r="B43" s="53"/>
-      <c r="C43" s="7" t="s">
+      <c r="A43" s="61"/>
+      <c r="B43" s="63"/>
+      <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="62"/>
-      <c r="E43" s="49"/>
-      <c r="F43" s="55"/>
-      <c r="G43" s="49"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="50"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="50" t="s">
+      <c r="A44" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="52" t="s">
+      <c r="B44" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="56" t="s">
+      <c r="D44" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="48" t="s">
+      <c r="E44" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="54" t="s">
+      <c r="F44" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="48" t="s">
+      <c r="G44" s="49" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="51"/>
-      <c r="B45" s="53"/>
-      <c r="C45" s="7" t="s">
+      <c r="A45" s="61"/>
+      <c r="B45" s="63"/>
+      <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="57"/>
-      <c r="E45" s="49"/>
-      <c r="F45" s="55"/>
-      <c r="G45" s="49"/>
+      <c r="D45" s="67"/>
+      <c r="E45" s="50"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="50"/>
       <c r="I45" s="1"/>
     </row>
     <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50" t="s">
+      <c r="A46" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="52" t="s">
+      <c r="B46" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="56" t="s">
+      <c r="D46" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="48" t="s">
+      <c r="E46" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="54" t="s">
+      <c r="F46" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="48" t="s">
+      <c r="G46" s="49" t="s">
         <v>84</v>
       </c>
       <c r="I46" s="1"/>
     </row>
     <row r="47" spans="1:9" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="51"/>
-      <c r="B47" s="53"/>
-      <c r="C47" s="7" t="s">
+      <c r="A47" s="61"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="57"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="58"/>
+      <c r="D47" s="67"/>
+      <c r="E47" s="50"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="68"/>
       <c r="I47" s="1"/>
     </row>
     <row r="48" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B48" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="18" t="s">
+      <c r="D48" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="41" t="s">
+      <c r="E48" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F48" s="42" t="s">
+      <c r="F48" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="46" t="s">
+      <c r="G48" s="43" t="s">
         <v>110</v>
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="9" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="38" t="s">
+      <c r="C49" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="D49" s="18" t="s">
+      <c r="D49" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="E49" s="41" t="s">
+      <c r="E49" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F49" s="42" t="s">
+      <c r="F49" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G49" s="45" t="s">
+      <c r="G49" s="42" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B50" s="13" t="s">
+      <c r="B50" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="7" t="s">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="41" t="s">
+      <c r="E50" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F50" s="42" t="s">
+      <c r="F50" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G50" s="44" t="s">
+      <c r="G50" s="41" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B51" s="13" t="s">
+      <c r="B51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="39" t="s">
+      <c r="C51" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="D51" s="18" t="s">
+      <c r="D51" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E51" s="41" t="s">
+      <c r="E51" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F51" s="42" t="s">
+      <c r="F51" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="G51" s="47" t="s">
+      <c r="G51" s="44" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B52" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="7">
+      <c r="C52" s="6">
         <v>32</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D52" s="6">
         <v>32</v>
       </c>
-      <c r="E52" s="41" t="s">
+      <c r="E52" s="38" t="s">
         <v>94</v>
       </c>
-      <c r="F52" s="15" t="s">
+      <c r="F52" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="G52" s="43" t="s">
+      <c r="G52" s="40" t="s">
         <v>96</v>
       </c>
       <c r="I52" s="1"/>
     </row>
     <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B53" s="13" t="s">
+      <c r="B53" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C53" s="6">
         <v>1234567890</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D53" s="6">
         <v>1234567890</v>
       </c>
-      <c r="E53" s="41" t="s">
+      <c r="E53" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="F53" s="15" t="s">
+      <c r="F53" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="G53" s="16" t="s">
+      <c r="G53" s="13" t="s">
         <v>98</v>
       </c>
       <c r="I53" s="1"/>
     </row>
     <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="37" t="s">
+      <c r="C54" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="E54" s="16" t="s">
+      <c r="E54" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="F54" s="15" t="s">
+      <c r="F54" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G54" s="16" t="s">
+      <c r="G54" s="13" t="s">
         <v>102</v>
       </c>
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="63" t="s">
+      <c r="A55" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="64"/>
-      <c r="C55" s="64"/>
-      <c r="D55" s="64"/>
-      <c r="E55" s="64"/>
-      <c r="F55" s="26" t="s">
+      <c r="B55" s="52"/>
+      <c r="C55" s="52"/>
+      <c r="D55" s="52"/>
+      <c r="E55" s="52"/>
+      <c r="F55" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G55" s="25" t="s">
+      <c r="G55" s="22" t="s">
         <v>15</v>
       </c>
       <c r="I55" s="1"/>
     </row>
     <row r="56" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="22" t="s">
+      <c r="A56" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B56" s="23" t="s">
+      <c r="B56" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C56" s="24" t="s">
+      <c r="C56" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D56" s="24" t="s">
+      <c r="D56" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="24" t="s">
+      <c r="E56" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F56" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G56" s="11" t="s">
+      <c r="G56" s="9" t="s">
         <v>0</v>
       </c>
       <c r="I56" s="1"/>
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
       <c r="E57" s="3"/>
-      <c r="F57" s="15"/>
+      <c r="F57" s="12"/>
       <c r="G57" s="3"/>
       <c r="I57" s="1"/>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B58" s="13" t="s">
+      <c r="B58" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
       <c r="E58" s="3"/>
-      <c r="F58" s="15"/>
+      <c r="F58" s="12"/>
       <c r="G58" s="3"/>
       <c r="I58" s="1"/>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
       <c r="E59" s="3"/>
-      <c r="F59" s="15"/>
+      <c r="F59" s="12"/>
       <c r="G59" s="3"/>
       <c r="I59" s="1"/>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="13" t="s">
+      <c r="B60" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7"/>
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
       <c r="E60" s="3"/>
-      <c r="F60" s="15"/>
+      <c r="F60" s="12"/>
       <c r="G60" s="3"/>
       <c r="I60" s="1"/>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="13" t="s">
+      <c r="B61" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
       <c r="E61" s="3"/>
-      <c r="F61" s="15"/>
+      <c r="F61" s="12"/>
       <c r="G61" s="3"/>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="13" t="s">
+      <c r="B62" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
       <c r="E62" s="3"/>
-      <c r="F62" s="15"/>
+      <c r="F62" s="12"/>
       <c r="G62" s="3"/>
       <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="13" t="s">
+      <c r="B63" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="7"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
       <c r="E63" s="3"/>
-      <c r="F63" s="15"/>
+      <c r="F63" s="12"/>
       <c r="G63" s="3"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="7"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
       <c r="E64" s="3"/>
-      <c r="F64" s="15"/>
+      <c r="F64" s="12"/>
       <c r="G64" s="3"/>
     </row>
     <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="13" t="s">
+      <c r="B65" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="7"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
       <c r="E65" s="3"/>
-      <c r="F65" s="15"/>
+      <c r="F65" s="12"/>
       <c r="G65" s="3"/>
     </row>
     <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="13" t="s">
+      <c r="B66" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="15"/>
-      <c r="G66" s="3"/>
+      <c r="C66" s="69">
+        <v>-987654321</v>
+      </c>
+      <c r="D66" s="69">
+        <v>-987654321</v>
+      </c>
+      <c r="E66" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" s="70" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="13" t="s">
+      <c r="B67" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="7"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="15"/>
-      <c r="G67" s="3"/>
-    </row>
-    <row r="68" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="14" t="s">
+      <c r="C67" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D67" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="E67" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F67" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G67" s="70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="13" t="s">
+      <c r="B68" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C68" s="34" t="s">
+        <v>115</v>
+      </c>
+      <c r="D68" s="69" t="s">
+        <v>115</v>
+      </c>
+      <c r="E68" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="F68" s="71" t="s">
+        <v>34</v>
+      </c>
+      <c r="G68" s="70" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="8"/>
-      <c r="E68" s="4"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="4"/>
+      <c r="C69" s="72">
+        <v>2147483648</v>
+      </c>
+      <c r="D69" s="72">
+        <v>2147483648</v>
+      </c>
+      <c r="E69" s="73">
+        <v>2147483647</v>
+      </c>
+      <c r="F69" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="G69" s="75" t="s">
+        <v>119</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="E38:E39"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A55:E55"/>
@@ -3628,36 +3729,18 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{256EE760-E688-4C56-B416-E0BCCD36032A}"/>
@@ -3680,7 +3763,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Uploading source code, test case output of Manipulating module and updating test case excel file of version 3
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
+++ b/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vansh\Documents\GitHub\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HET SEM-1\CPR 101\Final project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B326D33-3896-48DC-B619-EF8E5576CF35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0882F9-D1F6-4FC0-B546-C77465C95F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="142">
   <si>
     <t>Comments</t>
   </si>
@@ -1231,6 +1231,72 @@
   </si>
   <si>
     <t>Trying the edge values</t>
+  </si>
+  <si>
+    <t>hello, friend!</t>
+  </si>
+  <si>
+    <t>'friend' found at 7 position</t>
+  </si>
+  <si>
+    <t>Basic functionality test</t>
+  </si>
+  <si>
+    <t>friend</t>
+  </si>
+  <si>
+    <t>The cute brown cat</t>
+  </si>
+  <si>
+    <t>'cute' found at 4 position</t>
+  </si>
+  <si>
+    <t>Simple substring at the start</t>
+  </si>
+  <si>
+    <t>cute</t>
+  </si>
+  <si>
+    <t>zzzzzzzzzzzzzzzzzzzz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">'zz' found at 0 position </t>
+  </si>
+  <si>
+    <t>Checks multiple occurrences</t>
+  </si>
+  <si>
+    <t>zz</t>
+  </si>
+  <si>
+    <t>Special!@#characters*&amp;</t>
+  </si>
+  <si>
+    <t>@#characters' found at 8 position</t>
+  </si>
+  <si>
+    <t>Handling of special characters and symbols</t>
+  </si>
+  <si>
+    <t>@#characters</t>
+  </si>
+  <si>
+    <t>-  typical case</t>
+  </si>
+  <si>
+    <t>hello, world!</t>
+  </si>
+  <si>
+    <t>'World' found at 7 position</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>The search is case-sensitive. To fix this, make the search case-insensitive.</t>
+  </si>
+  <si>
+    <t>World</t>
   </si>
 </sst>
 </file>
@@ -1778,7 +1844,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1902,22 +1968,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1947,53 +2061,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2284,21 +2356,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D56" zoomScale="115" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D85" sqref="D85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.54296875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.90625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2309,22 +2381,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="67" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="52"/>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
       <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
@@ -2332,7 +2404,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2356,7 +2428,7 @@
       </c>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -2380,7 +2452,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -2404,7 +2476,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
@@ -2429,7 +2501,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
@@ -2453,7 +2525,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -2477,7 +2549,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2511,16 +2583,16 @@
       <c r="C10" s="6">
         <v>123456</v>
       </c>
-      <c r="D10" s="55" t="s">
+      <c r="D10" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="58" t="s">
+      <c r="E10" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="47" t="s">
+      <c r="G10" s="63" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
@@ -2531,10 +2603,10 @@
       <c r="C11" s="4">
         <v>7891011</v>
       </c>
-      <c r="D11" s="56"/>
-      <c r="E11" s="59"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="48"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="64"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2547,16 +2619,16 @@
       <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="45" t="s">
+      <c r="F12" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="47" t="s">
+      <c r="G12" s="63" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
@@ -2567,10 +2639,10 @@
       <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="59"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="48"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="64"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2583,16 +2655,16 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="55" t="s">
+      <c r="D14" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="74" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="47" t="s">
+      <c r="G14" s="63" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
@@ -2603,13 +2675,13 @@
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="56"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="46"/>
-      <c r="G15" s="48"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="64"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
@@ -2619,33 +2691,33 @@
       <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="47" t="s">
+      <c r="E16" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="49" t="s">
+      <c r="G16" s="52" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="57"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="50"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="59"/>
+      <c r="G17" s="53"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
@@ -2653,29 +2725,29 @@
         <v>73</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="49" t="s">
+      <c r="D18" s="71"/>
+      <c r="E18" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="45" t="s">
+      <c r="F18" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="47" t="s">
+      <c r="G18" s="63" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="56"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="46"/>
-      <c r="G19" s="48"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="64"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
@@ -2685,31 +2757,31 @@
       <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="55" t="s">
+      <c r="D20" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="49" t="s">
+      <c r="E20" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="47" t="s">
+      <c r="G20" s="63" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="56"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="46"/>
-      <c r="G21" s="48"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="64"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="50" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
@@ -2733,7 +2805,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="193.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>4</v>
       </c>
@@ -2757,7 +2829,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2781,7 +2853,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
@@ -2805,7 +2877,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
@@ -2829,7 +2901,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +2925,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
@@ -2877,7 +2949,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
@@ -2901,7 +2973,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>3</v>
       </c>
@@ -2925,7 +2997,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
@@ -2949,7 +3021,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
@@ -2974,13 +3046,13 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="51" t="s">
+      <c r="A33" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="52"/>
-      <c r="C33" s="52"/>
-      <c r="D33" s="52"/>
-      <c r="E33" s="52"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
       <c r="F33" s="23" t="s">
         <v>2</v>
       </c>
@@ -2988,7 +3060,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
@@ -3011,7 +3083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
@@ -3035,7 +3107,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
@@ -3059,7 +3131,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
@@ -3083,187 +3155,187 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="60" t="s">
+    <row r="38" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="62" t="s">
+      <c r="B38" s="56" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="60" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="E38" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="45" t="s">
+      <c r="F38" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="47" t="s">
+      <c r="G38" s="63" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61"/>
-      <c r="B39" s="63"/>
+    <row r="39" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="55"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="6">
         <v>3</v>
       </c>
-      <c r="D39" s="65"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="48"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="64"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="60" t="s">
+    <row r="40" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="62" t="s">
+      <c r="B40" s="56" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="64" t="s">
+      <c r="D40" s="60" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="49" t="s">
+      <c r="E40" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="45" t="s">
+      <c r="F40" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="G40" s="63" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="61"/>
-      <c r="B41" s="63"/>
+    <row r="41" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="55"/>
+      <c r="B41" s="57"/>
       <c r="C41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="65"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="46"/>
-      <c r="G41" s="48"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="53"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="64"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="60" t="s">
+    <row r="42" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="62" t="s">
+      <c r="B42" s="56" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="49" t="s">
+      <c r="E42" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="45" t="s">
+      <c r="F42" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="49" t="s">
+      <c r="G42" s="52" t="s">
         <v>81</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="61"/>
-      <c r="B43" s="63"/>
+    <row r="43" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="55"/>
+      <c r="B43" s="57"/>
       <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="65"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="46"/>
-      <c r="G43" s="50"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="53"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="53"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="60" t="s">
+    <row r="44" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="62" t="s">
+      <c r="B44" s="56" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="64" t="s">
+      <c r="D44" s="60" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="49" t="s">
+      <c r="E44" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="45" t="s">
+      <c r="F44" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="49" t="s">
+      <c r="G44" s="52" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="61"/>
-      <c r="B45" s="63"/>
+    <row r="45" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="55"/>
+      <c r="B45" s="57"/>
       <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="67"/>
-      <c r="E45" s="50"/>
-      <c r="F45" s="46"/>
-      <c r="G45" s="50"/>
+      <c r="D45" s="61"/>
+      <c r="E45" s="53"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="53"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="60" t="s">
+    <row r="46" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="62" t="s">
+      <c r="B46" s="56" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="64" t="s">
+      <c r="D46" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="49" t="s">
+      <c r="E46" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="45" t="s">
+      <c r="F46" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="49" t="s">
+      <c r="G46" s="52" t="s">
         <v>84</v>
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="61"/>
-      <c r="B47" s="63"/>
+    <row r="47" spans="1:9" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="55"/>
+      <c r="B47" s="57"/>
       <c r="C47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="67"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="46"/>
-      <c r="G47" s="68"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="53"/>
+      <c r="F47" s="59"/>
+      <c r="G47" s="62"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="11" t="s">
         <v>4</v>
       </c>
@@ -3287,7 +3359,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>4</v>
       </c>
@@ -3310,7 +3382,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="25" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>4</v>
       </c>
@@ -3331,7 +3403,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="11" t="s">
         <v>4</v>
       </c>
@@ -3354,7 +3426,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -3378,7 +3450,7 @@
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -3402,7 +3474,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -3427,13 +3499,13 @@
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="51" t="s">
+      <c r="A55" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="52"/>
-      <c r="C55" s="52"/>
-      <c r="D55" s="52"/>
-      <c r="E55" s="52"/>
+      <c r="B55" s="68"/>
+      <c r="C55" s="68"/>
+      <c r="D55" s="68"/>
+      <c r="E55" s="68"/>
       <c r="F55" s="23" t="s">
         <v>2</v>
       </c>
@@ -3442,7 +3514,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>9</v>
       </c>
@@ -3466,7 +3538,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>6</v>
       </c>
@@ -3480,7 +3552,7 @@
       <c r="G57" s="3"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>6</v>
       </c>
@@ -3494,7 +3566,7 @@
       <c r="G58" s="3"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
@@ -3508,211 +3580,393 @@
       <c r="G59" s="3"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="11" t="s">
+    <row r="60" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D60" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="E60" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F60" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G60" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="I60" s="1"/>
+    </row>
+    <row r="61" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="55"/>
+      <c r="B61" s="57"/>
+      <c r="C61" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D61" s="66"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="59"/>
+      <c r="G61" s="53"/>
+      <c r="I61" s="1"/>
+    </row>
+    <row r="62" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D62" s="60" t="s">
+        <v>125</v>
+      </c>
+      <c r="E62" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F62" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G62" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="I62" s="1"/>
+    </row>
+    <row r="63" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="55"/>
+      <c r="B63" s="57"/>
+      <c r="C63" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="D63" s="61"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="59"/>
+      <c r="G63" s="53"/>
+    </row>
+    <row r="64" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B64" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="6"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="3"/>
-      <c r="I60" s="1"/>
-    </row>
-    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="11" t="s">
+      <c r="C64" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="D64" s="60" t="s">
+        <v>129</v>
+      </c>
+      <c r="E64" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="F64" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G64" s="52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="55"/>
+      <c r="B65" s="57"/>
+      <c r="C65" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D65" s="61"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="59"/>
+      <c r="G65" s="53"/>
+    </row>
+    <row r="66" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="B66" s="56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>132</v>
+      </c>
+      <c r="D66" s="56" t="s">
+        <v>133</v>
+      </c>
+      <c r="E66" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="F66" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" s="76" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="55"/>
+      <c r="B67" s="57"/>
+      <c r="C67" s="77" t="s">
+        <v>135</v>
+      </c>
+      <c r="D67" s="61"/>
+      <c r="E67" s="53"/>
+      <c r="F67" s="59"/>
+      <c r="G67" s="53"/>
+    </row>
+    <row r="68" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="54" t="s">
+        <v>5</v>
+      </c>
+      <c r="B68" s="56" t="s">
+        <v>136</v>
+      </c>
+      <c r="C68" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="D68" s="60" t="s">
+        <v>138</v>
+      </c>
+      <c r="E68" s="52" t="s">
+        <v>139</v>
+      </c>
+      <c r="F68" s="58" t="s">
+        <v>50</v>
+      </c>
+      <c r="G68" s="52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="55"/>
+      <c r="B69" s="57"/>
+      <c r="C69" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D69" s="61"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="59"/>
+      <c r="G69" s="53"/>
+    </row>
+    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="3"/>
+    </row>
+    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B71" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="3"/>
-      <c r="I61" s="1"/>
-    </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="11" t="s">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="3"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="3"/>
+    </row>
+    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="B72" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="3"/>
-      <c r="I62" s="1"/>
-    </row>
-    <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="11" t="s">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="3"/>
+    </row>
+    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="B73" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="3"/>
-    </row>
-    <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="3"/>
+    </row>
+    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="B74" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C64" s="6"/>
-      <c r="D64" s="6"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="3"/>
-    </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="11" t="s">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="3"/>
+    </row>
+    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B75" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C65" s="6"/>
-      <c r="D65" s="6"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="3"/>
-    </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="11" t="s">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="3"/>
+    </row>
+    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="B76" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C66" s="69">
+      <c r="C76" s="45">
         <v>-987654321</v>
       </c>
-      <c r="D66" s="69">
+      <c r="D76" s="45">
         <v>-987654321</v>
       </c>
-      <c r="E66" s="70" t="s">
+      <c r="E76" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="71" t="s">
+      <c r="F76" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="70" t="s">
+      <c r="G76" s="46" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="11" t="s">
+    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="B77" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C67" s="34" t="s">
+      <c r="C77" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="D67" s="34" t="s">
+      <c r="D77" s="34" t="s">
         <v>117</v>
       </c>
-      <c r="E67" s="70" t="s">
+      <c r="E77" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F67" s="71" t="s">
+      <c r="F77" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G67" s="70" t="s">
+      <c r="G77" s="46" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="11" t="s">
+    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A78" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B78" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C68" s="34" t="s">
+      <c r="C78" s="34" t="s">
         <v>115</v>
       </c>
-      <c r="D68" s="69" t="s">
+      <c r="D78" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="E68" s="70" t="s">
+      <c r="E78" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F68" s="71" t="s">
+      <c r="F78" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="G68" s="70" t="s">
+      <c r="G78" s="46" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
+    <row r="79" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="B79" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C69" s="72">
+      <c r="C79" s="48">
         <v>2147483648</v>
       </c>
-      <c r="D69" s="72">
+      <c r="D79" s="48">
         <v>2147483648</v>
       </c>
-      <c r="E69" s="73">
+      <c r="E79" s="49">
         <v>2147483647</v>
       </c>
-      <c r="F69" s="74" t="s">
+      <c r="F79" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="G69" s="75" t="s">
+      <c r="G79" s="51" t="s">
         <v>119</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="E38:E39"/>
+  <mergeCells count="88">
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A55:E55"/>
@@ -3729,18 +3983,36 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{256EE760-E688-4C56-B416-E0BCCD36032A}"/>
@@ -3757,9 +4029,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.5546875" customWidth="1"/>
+    <col min="1" max="1" width="89.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated test case excel file.
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
+++ b/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HET SEM-1\CPR 101\Final project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d68bcfb44c4b5b/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0882F9-D1F6-4FC0-B546-C77465C95F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{820A1A6D-C506-4431-9ED4-53A462521B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -774,7 +774,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="146">
   <si>
     <t>Comments</t>
   </si>
@@ -1297,6 +1297,18 @@
   </si>
   <si>
     <t>World</t>
+  </si>
+  <si>
+    <t>Manav$student98743@34324</t>
+  </si>
+  <si>
+    <t>Ontariokfj9438tfd@#$@$%</t>
+  </si>
+  <si>
+    <t>Toromntoof2935u467$%^&amp;</t>
+  </si>
+  <si>
+    <t>After each string is entered, it is copied to the "New destination string."</t>
   </si>
 </sst>
 </file>
@@ -1989,6 +2001,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2063,9 +2078,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2358,19 +2370,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8467BC1A-7E6C-461F-88DC-8200B861EB6B}">
   <dimension ref="A1:I79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="85" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="D85" sqref="D85"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.08984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.54296875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.90625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2381,22 +2393,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
     </row>
     <row r="2" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
@@ -2404,7 +2416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2428,7 +2440,7 @@
       </c>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -2452,7 +2464,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -2476,7 +2488,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
@@ -2501,7 +2513,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
@@ -2525,7 +2537,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -2549,7 +2561,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2583,16 +2595,16 @@
       <c r="C10" s="6">
         <v>123456</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="58" t="s">
+      <c r="F10" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
@@ -2603,10 +2615,10 @@
       <c r="C11" s="4">
         <v>7891011</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="64"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="65"/>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2619,16 +2631,16 @@
       <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="63" t="s">
+      <c r="G12" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
@@ -2639,10 +2651,10 @@
       <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="59"/>
-      <c r="G13" s="64"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="65"/>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2655,16 +2667,16 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="58" t="s">
+      <c r="F14" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="G14" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
@@ -2675,13 +2687,13 @@
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="64"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="65"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
@@ -2691,33 +2703,33 @@
       <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="63" t="s">
+      <c r="E16" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="58" t="s">
+      <c r="F16" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="52" t="s">
+      <c r="G16" s="53" t="s">
         <v>53</v>
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="64"/>
-      <c r="F17" s="59"/>
-      <c r="G17" s="53"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="54"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
@@ -2725,29 +2737,29 @@
         <v>73</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="71"/>
-      <c r="E18" s="52" t="s">
+      <c r="D18" s="72"/>
+      <c r="E18" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="58" t="s">
+      <c r="F18" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="63" t="s">
+      <c r="G18" s="64" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="35" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="72"/>
-      <c r="E19" s="53"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="64"/>
+      <c r="D19" s="73"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="65"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
@@ -2757,31 +2769,31 @@
       <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="72" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="E20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="64" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="72"/>
-      <c r="E21" s="53"/>
-      <c r="F21" s="59"/>
-      <c r="G21" s="64"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="65"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="50" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
@@ -2805,7 +2817,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="193.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>4</v>
       </c>
@@ -2829,7 +2841,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2853,7 +2865,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
@@ -2877,7 +2889,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
@@ -2901,7 +2913,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
@@ -2925,7 +2937,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
@@ -2949,7 +2961,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
@@ -2973,7 +2985,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>3</v>
       </c>
@@ -2997,7 +3009,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
@@ -3021,7 +3033,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
@@ -3046,13 +3058,13 @@
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="23" t="s">
         <v>2</v>
       </c>
@@ -3060,7 +3072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
@@ -3083,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
@@ -3107,7 +3119,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="15.5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
@@ -3131,7 +3143,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
@@ -3155,187 +3167,187 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="54" t="s">
+    <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="57" t="s">
         <v>74</v>
       </c>
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="60" t="s">
+      <c r="D38" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="52" t="s">
+      <c r="E38" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="58" t="s">
+      <c r="F38" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="63" t="s">
+      <c r="G38" s="64" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
-      <c r="B39" s="57"/>
+    <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="56"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="6">
         <v>3</v>
       </c>
-      <c r="D39" s="66"/>
-      <c r="E39" s="53"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="64"/>
+      <c r="D39" s="67"/>
+      <c r="E39" s="54"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="65"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="54" t="s">
+    <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B40" s="56" t="s">
+      <c r="B40" s="57" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="60" t="s">
+      <c r="D40" s="61" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="52" t="s">
+      <c r="E40" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="58" t="s">
+      <c r="F40" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="63" t="s">
+      <c r="G40" s="64" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="55"/>
-      <c r="B41" s="57"/>
+    <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="56"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="53"/>
-      <c r="F41" s="59"/>
-      <c r="G41" s="64"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="65"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="54" t="s">
+    <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="56" t="s">
+      <c r="B42" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="65" t="s">
+      <c r="D42" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="E42" s="52" t="s">
+      <c r="E42" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="58" t="s">
+      <c r="F42" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="52" t="s">
+      <c r="G42" s="53" t="s">
         <v>81</v>
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="55"/>
-      <c r="B43" s="57"/>
+    <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="66"/>
-      <c r="E43" s="53"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="53"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="54"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="54"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="54" t="s">
+    <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C44" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="60" t="s">
+      <c r="D44" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="E44" s="52" t="s">
+      <c r="E44" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="58" t="s">
+      <c r="F44" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G44" s="52" t="s">
+      <c r="G44" s="53" t="s">
         <v>81</v>
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="55"/>
-      <c r="B45" s="57"/>
+    <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="56"/>
+      <c r="B45" s="58"/>
       <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="61"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="59"/>
-      <c r="G45" s="53"/>
+      <c r="D45" s="62"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="54"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="54" t="s">
+    <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B46" s="56" t="s">
+      <c r="B46" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="60" t="s">
+      <c r="D46" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="E46" s="52" t="s">
+      <c r="E46" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="58" t="s">
+      <c r="F46" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G46" s="52" t="s">
+      <c r="G46" s="53" t="s">
         <v>84</v>
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="55"/>
-      <c r="B47" s="57"/>
+    <row r="47" spans="1:9" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="56"/>
+      <c r="B47" s="58"/>
       <c r="C47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="61"/>
-      <c r="E47" s="53"/>
-      <c r="F47" s="59"/>
-      <c r="G47" s="62"/>
+      <c r="D47" s="62"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="63"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="50.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>4</v>
       </c>
@@ -3359,7 +3371,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>4</v>
       </c>
@@ -3382,7 +3394,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>4</v>
       </c>
@@ -3403,7 +3415,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>4</v>
       </c>
@@ -3426,7 +3438,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -3450,7 +3462,7 @@
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -3474,7 +3486,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -3499,13 +3511,13 @@
       <c r="I54" s="1"/>
     </row>
     <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="67" t="s">
+      <c r="A55" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="23" t="s">
         <v>2</v>
       </c>
@@ -3514,7 +3526,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>9</v>
       </c>
@@ -3538,222 +3550,232 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="E57" s="3"/>
       <c r="F57" s="12"/>
       <c r="G57" s="3"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B58" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
+      <c r="C58" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>145</v>
+      </c>
       <c r="E58" s="3"/>
       <c r="F58" s="12"/>
       <c r="G58" s="3"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C59" s="6"/>
+        <v>20</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>144</v>
+      </c>
       <c r="D59" s="6"/>
       <c r="E59" s="3"/>
       <c r="F59" s="12"/>
       <c r="G59" s="3"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="54" t="s">
+    <row r="60" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="60" t="s">
+      <c r="D60" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="E60" s="52" t="s">
+      <c r="E60" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F60" s="58" t="s">
+      <c r="F60" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G60" s="52" t="s">
+      <c r="G60" s="53" t="s">
         <v>122</v>
       </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
-      <c r="B61" s="57"/>
+    <row r="61" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="56"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="66"/>
-      <c r="E61" s="53"/>
-      <c r="F61" s="59"/>
-      <c r="G61" s="53"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="54"/>
+      <c r="F61" s="60"/>
+      <c r="G61" s="54"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="54" t="s">
+    <row r="62" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="57" t="s">
         <v>20</v>
       </c>
       <c r="C62" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D62" s="60" t="s">
+      <c r="D62" s="61" t="s">
         <v>125</v>
       </c>
-      <c r="E62" s="52" t="s">
+      <c r="E62" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F62" s="58" t="s">
+      <c r="F62" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G62" s="52" t="s">
+      <c r="G62" s="53" t="s">
         <v>126</v>
       </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="55"/>
-      <c r="B63" s="57"/>
+    <row r="63" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="56"/>
+      <c r="B63" s="58"/>
       <c r="C63" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="61"/>
-      <c r="E63" s="53"/>
-      <c r="F63" s="59"/>
-      <c r="G63" s="53"/>
-    </row>
-    <row r="64" spans="1:9" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="54" t="s">
+      <c r="D63" s="62"/>
+      <c r="E63" s="54"/>
+      <c r="F63" s="60"/>
+      <c r="G63" s="54"/>
+    </row>
+    <row r="64" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="57" t="s">
         <v>19</v>
       </c>
       <c r="C64" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="60" t="s">
+      <c r="D64" s="61" t="s">
         <v>129</v>
       </c>
-      <c r="E64" s="52" t="s">
+      <c r="E64" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="58" t="s">
+      <c r="F64" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G64" s="52" t="s">
+      <c r="G64" s="53" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="55"/>
-      <c r="B65" s="57"/>
+    <row r="65" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="56"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D65" s="61"/>
-      <c r="E65" s="53"/>
-      <c r="F65" s="59"/>
-      <c r="G65" s="53"/>
-    </row>
-    <row r="66" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="54" t="s">
+      <c r="D65" s="62"/>
+      <c r="E65" s="54"/>
+      <c r="F65" s="60"/>
+      <c r="G65" s="54"/>
+    </row>
+    <row r="66" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="57" t="s">
         <v>21</v>
       </c>
       <c r="C66" t="s">
         <v>132</v>
       </c>
-      <c r="D66" s="56" t="s">
+      <c r="D66" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="E66" s="76" t="s">
+      <c r="E66" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="58" t="s">
+      <c r="F66" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="76" t="s">
+      <c r="G66" s="77" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
-      <c r="B67" s="57"/>
-      <c r="C67" s="77" t="s">
+    <row r="67" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="56"/>
+      <c r="B67" s="58"/>
+      <c r="C67" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="61"/>
-      <c r="E67" s="53"/>
-      <c r="F67" s="59"/>
-      <c r="G67" s="53"/>
-    </row>
-    <row r="68" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="54" t="s">
+      <c r="D67" s="62"/>
+      <c r="E67" s="54"/>
+      <c r="F67" s="60"/>
+      <c r="G67" s="54"/>
+    </row>
+    <row r="68" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="57" t="s">
         <v>136</v>
       </c>
       <c r="C68" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D68" s="60" t="s">
+      <c r="D68" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="E68" s="52" t="s">
+      <c r="E68" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F68" s="58" t="s">
+      <c r="F68" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G68" s="52" t="s">
+      <c r="G68" s="53" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
-      <c r="B69" s="57"/>
+    <row r="69" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="56"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="61"/>
-      <c r="E69" s="53"/>
-      <c r="F69" s="59"/>
-      <c r="G69" s="53"/>
-    </row>
-    <row r="70" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="D69" s="62"/>
+      <c r="E69" s="54"/>
+      <c r="F69" s="60"/>
+      <c r="G69" s="54"/>
+    </row>
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>5</v>
       </c>
@@ -3766,7 +3788,7 @@
       <c r="F70" s="12"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>5</v>
       </c>
@@ -3779,7 +3801,7 @@
       <c r="F71" s="12"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>5</v>
       </c>
@@ -3792,7 +3814,7 @@
       <c r="F72" s="12"/>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>4</v>
       </c>
@@ -3805,7 +3827,7 @@
       <c r="F73" s="12"/>
       <c r="G73" s="3"/>
     </row>
-    <row r="74" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>4</v>
       </c>
@@ -3818,7 +3840,7 @@
       <c r="F74" s="12"/>
       <c r="G74" s="3"/>
     </row>
-    <row r="75" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>4</v>
       </c>
@@ -3831,7 +3853,7 @@
       <c r="F75" s="12"/>
       <c r="G75" s="3"/>
     </row>
-    <row r="76" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>3</v>
       </c>
@@ -3854,7 +3876,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>3</v>
       </c>
@@ -3877,7 +3899,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>3</v>
       </c>
@@ -3900,7 +3922,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="11" t="s">
         <v>3</v>
       </c>
@@ -4016,10 +4038,12 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{256EE760-E688-4C56-B416-E0BCCD36032A}"/>
+    <hyperlink ref="C57" r:id="rId2" xr:uid="{0420C53A-3C14-45B7-B506-7AE1137469DC}"/>
+    <hyperlink ref="C58" r:id="rId3" xr:uid="{D74ECD77-C3DF-43FC-8395-B5848CF26889}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <legacyDrawing r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -4029,9 +4053,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.54296875" customWidth="1"/>
+    <col min="1" max="1" width="89.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to test cases excel file
</commit_message>
<xml_diff>
--- a/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
+++ b/Documents/Test cases/Version 3/Final-Project-Test-Cases-version-3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca cpp\CPR101\group project\CPR101_Group_41_2024Final_Project\Documents\Test cases\Version 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b6d68bcfb44c4b5b/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA2FDE6-174A-4C34-AD53-F265EF49363A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="7" r:id="rId1"/>
@@ -2022,30 +2022,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2073,10 +2076,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2374,18 +2374,18 @@
       <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5546875" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="65.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="65.88671875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>1</v>
       </c>
@@ -2393,22 +2393,22 @@
         <f t="array" aca="1" ref="B1" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,255)</f>
         <v>main</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="70" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
-      <c r="F1" s="70"/>
-      <c r="G1" s="70"/>
-    </row>
-    <row r="2" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+    </row>
+    <row r="2" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
       <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>9</v>
       </c>
@@ -2440,7 +2440,7 @@
       </c>
       <c r="H3" s="18"/>
     </row>
-    <row r="4" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>6</v>
       </c>
@@ -2464,7 +2464,7 @@
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>6</v>
       </c>
@@ -2488,7 +2488,7 @@
       </c>
       <c r="I5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
@@ -2513,7 +2513,7 @@
       <c r="H6" s="18"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
@@ -2537,7 +2537,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -2561,7 +2561,7 @@
       </c>
       <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>6</v>
       </c>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="I9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>5</v>
       </c>
@@ -2595,33 +2595,33 @@
       <c r="C10" s="6">
         <v>123456</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="72" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="74" t="s">
+      <c r="E10" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="61" t="s">
+      <c r="F10" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="65" t="s">
+      <c r="G10" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I10" s="1"/>
     </row>
-    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="10"/>
       <c r="C11" s="4">
         <v>7891011</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="62"/>
-      <c r="G11" s="66"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="60"/>
+      <c r="G11" s="65"/>
       <c r="I11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>5</v>
       </c>
@@ -2631,33 +2631,33 @@
       <c r="C12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="74" t="s">
+      <c r="E12" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="61" t="s">
+      <c r="F12" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="65" t="s">
+      <c r="G12" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I12" s="1"/>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11"/>
       <c r="B13" s="10"/>
       <c r="C13" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D13" s="72"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="62"/>
-      <c r="G13" s="66"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="76"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="65"/>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>5</v>
       </c>
@@ -2667,33 +2667,33 @@
       <c r="C14" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="74" t="s">
+      <c r="E14" s="75" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="61" t="s">
+      <c r="F14" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="65" t="s">
+      <c r="G14" s="64" t="s">
         <v>35</v>
       </c>
       <c r="I14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="10"/>
       <c r="C15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="72"/>
-      <c r="E15" s="75"/>
-      <c r="F15" s="62"/>
-      <c r="G15" s="66"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="76"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="65"/>
       <c r="I15" s="1"/>
     </row>
-    <row r="16" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>5</v>
       </c>
@@ -2703,13 +2703,13 @@
       <c r="C16" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="73" t="s">
+      <c r="D16" s="74" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="65" t="s">
+      <c r="E16" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="61" t="s">
+      <c r="F16" s="59" t="s">
         <v>50</v>
       </c>
       <c r="G16" s="53" t="s">
@@ -2717,19 +2717,19 @@
       </c>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="10"/>
       <c r="C17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="73"/>
-      <c r="E17" s="66"/>
-      <c r="F17" s="62"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="60"/>
       <c r="G17" s="54"/>
       <c r="I17" s="1"/>
     </row>
-    <row r="18" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
@@ -2737,29 +2737,29 @@
         <v>73</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="71"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="61" t="s">
+      <c r="F18" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="65" t="s">
+      <c r="G18" s="64" t="s">
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
     </row>
-    <row r="19" spans="1:9" ht="34.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11"/>
       <c r="B19" s="10"/>
       <c r="C19" s="6"/>
-      <c r="D19" s="72"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="54"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="66"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="65"/>
       <c r="I19" s="1"/>
     </row>
-    <row r="20" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>5</v>
       </c>
@@ -2769,31 +2769,31 @@
       <c r="C20" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="72" t="s">
         <v>46</v>
       </c>
       <c r="E20" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="61" t="s">
+      <c r="F20" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="65" t="s">
+      <c r="G20" s="64" t="s">
         <v>51</v>
       </c>
       <c r="I20" s="1"/>
     </row>
-    <row r="21" spans="1:9" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="10"/>
       <c r="C21" s="6"/>
-      <c r="D21" s="72"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="54"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="66"/>
+      <c r="F21" s="60"/>
+      <c r="G21" s="65"/>
       <c r="I21" s="1"/>
     </row>
-    <row r="22" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>4</v>
       </c>
@@ -2817,7 +2817,7 @@
       </c>
       <c r="I22" s="1"/>
     </row>
-    <row r="23" spans="1:9" ht="193.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" ht="193.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>4</v>
       </c>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="I23" s="1"/>
     </row>
-    <row r="24" spans="1:9" ht="143.44999999999999" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" ht="143.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>4</v>
       </c>
@@ -2865,7 +2865,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>3</v>
       </c>
@@ -2889,7 +2889,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>3</v>
       </c>
@@ -2937,7 +2937,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>3</v>
       </c>
@@ -2985,7 +2985,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>3</v>
       </c>
@@ -3009,7 +3009,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>3</v>
       </c>
@@ -3033,7 +3033,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>3</v>
       </c>
@@ -3057,14 +3057,14 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+    <row r="33" spans="1:9" s="7" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="68"/>
-      <c r="C33" s="68"/>
-      <c r="D33" s="68"/>
-      <c r="E33" s="68"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
       <c r="F33" s="23" t="s">
         <v>2</v>
       </c>
@@ -3072,7 +3072,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="19" t="s">
         <v>9</v>
       </c>
@@ -3095,7 +3095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>6</v>
       </c>
@@ -3119,7 +3119,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>6</v>
       </c>
@@ -3143,7 +3143,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>6</v>
       </c>
@@ -3167,7 +3167,7 @@
       </c>
       <c r="I37" s="1"/>
     </row>
-    <row r="38" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="55" t="s">
         <v>5</v>
       </c>
@@ -3177,33 +3177,33 @@
       <c r="C38" s="6">
         <v>1</v>
       </c>
-      <c r="D38" s="59" t="s">
+      <c r="D38" s="61" t="s">
         <v>75</v>
       </c>
       <c r="E38" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F38" s="61" t="s">
+      <c r="F38" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G38" s="65" t="s">
+      <c r="G38" s="64" t="s">
         <v>85</v>
       </c>
       <c r="I38" s="1"/>
     </row>
-    <row r="39" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="56"/>
       <c r="B39" s="58"/>
       <c r="C39" s="6">
         <v>3</v>
       </c>
-      <c r="D39" s="64"/>
+      <c r="D39" s="67"/>
       <c r="E39" s="54"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="66"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="65"/>
       <c r="I39" s="1"/>
     </row>
-    <row r="40" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="55" t="s">
         <v>5</v>
       </c>
@@ -3213,33 +3213,33 @@
       <c r="C40" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="61" t="s">
         <v>78</v>
       </c>
       <c r="E40" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F40" s="61" t="s">
+      <c r="F40" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G40" s="65" t="s">
+      <c r="G40" s="64" t="s">
         <v>86</v>
       </c>
       <c r="I40" s="1"/>
     </row>
-    <row r="41" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
       <c r="B41" s="58"/>
       <c r="C41" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D41" s="64"/>
+      <c r="D41" s="67"/>
       <c r="E41" s="54"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="66"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="65"/>
       <c r="I41" s="1"/>
     </row>
-    <row r="42" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="55" t="s">
         <v>5</v>
       </c>
@@ -3249,13 +3249,13 @@
       <c r="C42" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D42" s="76" t="s">
+      <c r="D42" s="66" t="s">
         <v>80</v>
       </c>
       <c r="E42" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F42" s="61" t="s">
+      <c r="F42" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G42" s="53" t="s">
@@ -3263,19 +3263,19 @@
       </c>
       <c r="I42" s="1"/>
     </row>
-    <row r="43" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="56"/>
       <c r="B43" s="58"/>
       <c r="C43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D43" s="64"/>
+      <c r="D43" s="67"/>
       <c r="E43" s="54"/>
-      <c r="F43" s="62"/>
+      <c r="F43" s="60"/>
       <c r="G43" s="54"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="55" t="s">
         <v>5</v>
       </c>
@@ -3285,13 +3285,13 @@
       <c r="C44" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D44" s="59" t="s">
+      <c r="D44" s="61" t="s">
         <v>82</v>
       </c>
       <c r="E44" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F44" s="61" t="s">
+      <c r="F44" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G44" s="53" t="s">
@@ -3299,19 +3299,19 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="56"/>
       <c r="B45" s="58"/>
       <c r="C45" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="60"/>
+      <c r="D45" s="62"/>
       <c r="E45" s="54"/>
-      <c r="F45" s="62"/>
+      <c r="F45" s="60"/>
       <c r="G45" s="54"/>
       <c r="I45" s="1"/>
     </row>
-    <row r="46" spans="1:9" ht="15.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" ht="15.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="55" t="s">
         <v>5</v>
       </c>
@@ -3321,13 +3321,13 @@
       <c r="C46" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D46" s="59" t="s">
+      <c r="D46" s="61" t="s">
         <v>83</v>
       </c>
       <c r="E46" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F46" s="61" t="s">
+      <c r="F46" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G46" s="53" t="s">
@@ -3335,19 +3335,19 @@
       </c>
       <c r="I46" s="1"/>
     </row>
-    <row r="47" spans="1:9" ht="15.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="15.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="56"/>
       <c r="B47" s="58"/>
       <c r="C47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="60"/>
+      <c r="D47" s="62"/>
       <c r="E47" s="54"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="77"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="63"/>
       <c r="I47" s="1"/>
     </row>
-    <row r="48" spans="1:9" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="11" t="s">
         <v>4</v>
       </c>
@@ -3371,7 +3371,7 @@
       </c>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" s="7" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>4</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>4</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="11" t="s">
         <v>4</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>3</v>
       </c>
@@ -3462,7 +3462,7 @@
       </c>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>3</v>
       </c>
@@ -3486,7 +3486,7 @@
       </c>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>3</v>
       </c>
@@ -3510,14 +3510,14 @@
       </c>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="67" t="s">
+    <row r="55" spans="1:9" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B55" s="68"/>
-      <c r="C55" s="68"/>
-      <c r="D55" s="68"/>
-      <c r="E55" s="68"/>
+      <c r="B55" s="69"/>
+      <c r="C55" s="69"/>
+      <c r="D55" s="69"/>
+      <c r="E55" s="69"/>
       <c r="F55" s="23" t="s">
         <v>2</v>
       </c>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="19" t="s">
         <v>9</v>
       </c>
@@ -3550,7 +3550,7 @@
       </c>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A57" s="11" t="s">
         <v>6</v>
       </c>
@@ -3568,7 +3568,7 @@
       <c r="G57" s="3"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A58" s="11" t="s">
         <v>6</v>
       </c>
@@ -3586,7 +3586,7 @@
       <c r="G58" s="3"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="11" t="s">
         <v>6</v>
       </c>
@@ -3602,7 +3602,7 @@
       <c r="G59" s="3"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="55" t="s">
         <v>5</v>
       </c>
@@ -3612,13 +3612,13 @@
       <c r="C60" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D60" s="59" t="s">
+      <c r="D60" s="61" t="s">
         <v>121</v>
       </c>
       <c r="E60" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F60" s="61" t="s">
+      <c r="F60" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G60" s="53" t="s">
@@ -3626,19 +3626,19 @@
       </c>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="56"/>
       <c r="B61" s="58"/>
       <c r="C61" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="D61" s="64"/>
+      <c r="D61" s="67"/>
       <c r="E61" s="54"/>
-      <c r="F61" s="62"/>
+      <c r="F61" s="60"/>
       <c r="G61" s="54"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="55" t="s">
         <v>5</v>
       </c>
@@ -3648,13 +3648,13 @@
       <c r="C62" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="D62" s="59" t="s">
+      <c r="D62" s="61" t="s">
         <v>125</v>
       </c>
       <c r="E62" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F62" s="61" t="s">
+      <c r="F62" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G62" s="53" t="s">
@@ -3662,18 +3662,18 @@
       </c>
       <c r="I62" s="1"/>
     </row>
-    <row r="63" spans="1:9" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="56"/>
       <c r="B63" s="58"/>
       <c r="C63" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D63" s="60"/>
+      <c r="D63" s="62"/>
       <c r="E63" s="54"/>
-      <c r="F63" s="62"/>
+      <c r="F63" s="60"/>
       <c r="G63" s="54"/>
     </row>
-    <row r="64" spans="1:9" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="55" t="s">
         <v>5</v>
       </c>
@@ -3683,31 +3683,31 @@
       <c r="C64" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="D64" s="59" t="s">
+      <c r="D64" s="61" t="s">
         <v>129</v>
       </c>
       <c r="E64" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="F64" s="61" t="s">
+      <c r="F64" s="59" t="s">
         <v>34</v>
       </c>
       <c r="G64" s="53" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="56"/>
       <c r="B65" s="58"/>
       <c r="C65" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="D65" s="60"/>
+      <c r="D65" s="62"/>
       <c r="E65" s="54"/>
-      <c r="F65" s="62"/>
+      <c r="F65" s="60"/>
       <c r="G65" s="54"/>
     </row>
-    <row r="66" spans="1:7" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="55" t="s">
         <v>5</v>
       </c>
@@ -3720,28 +3720,28 @@
       <c r="D66" s="57" t="s">
         <v>133</v>
       </c>
-      <c r="E66" s="63" t="s">
+      <c r="E66" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="F66" s="61" t="s">
+      <c r="F66" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="63" t="s">
+      <c r="G66" s="77" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="56"/>
       <c r="B67" s="58"/>
       <c r="C67" s="52" t="s">
         <v>135</v>
       </c>
-      <c r="D67" s="60"/>
+      <c r="D67" s="62"/>
       <c r="E67" s="54"/>
-      <c r="F67" s="62"/>
+      <c r="F67" s="60"/>
       <c r="G67" s="54"/>
     </row>
-    <row r="68" spans="1:7" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="55" t="s">
         <v>5</v>
       </c>
@@ -3751,31 +3751,31 @@
       <c r="C68" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D68" s="59" t="s">
+      <c r="D68" s="61" t="s">
         <v>138</v>
       </c>
       <c r="E68" s="53" t="s">
         <v>139</v>
       </c>
-      <c r="F68" s="61" t="s">
+      <c r="F68" s="59" t="s">
         <v>50</v>
       </c>
       <c r="G68" s="53" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="12.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" ht="12.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="56"/>
       <c r="B69" s="58"/>
       <c r="C69" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D69" s="60"/>
+      <c r="D69" s="62"/>
       <c r="E69" s="54"/>
-      <c r="F69" s="62"/>
+      <c r="F69" s="60"/>
       <c r="G69" s="54"/>
     </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>4</v>
       </c>
@@ -3788,7 +3788,7 @@
       <c r="F70" s="12"/>
       <c r="G70" s="3"/>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
         <v>4</v>
       </c>
@@ -3801,7 +3801,7 @@
       <c r="F71" s="12"/>
       <c r="G71" s="3"/>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
         <v>4</v>
       </c>
@@ -3814,7 +3814,7 @@
       <c r="F72" s="12"/>
       <c r="G72" s="3"/>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
         <v>3</v>
       </c>
@@ -3837,7 +3837,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>3</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>3</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="11" t="s">
         <v>3</v>
       </c>
@@ -3908,36 +3908,48 @@
     </row>
   </sheetData>
   <mergeCells count="88">
-    <mergeCell ref="G44:G45"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="D44:D45"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="F42:F43"/>
-    <mergeCell ref="G42:G43"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="F38:F39"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="A68:A69"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="F18:F19"/>
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A55:E55"/>
@@ -3954,48 +3966,36 @@
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="F38:F39"/>
+    <mergeCell ref="G38:G39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="G40:G41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="F42:F43"/>
+    <mergeCell ref="G42:G43"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="G44:G45"/>
+    <mergeCell ref="A46:A47"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C36" r:id="rId1" xr:uid="{256EE760-E688-4C56-B416-E0BCCD36032A}"/>
@@ -4014,12 +4014,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.5703125" customWidth="1"/>
+    <col min="1" max="1" width="89.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>10</v>
       </c>

</xml_diff>